<commit_message>
Data 3 eingefügt, MemoryTracer macht Fehler
</commit_message>
<xml_diff>
--- a/Aufgabenliste.xlsx
+++ b/Aufgabenliste.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,6 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\workspace\JavaMemoryTracerAufgaben\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B13ED5-6AC7-47DD-A8AF-FDD1CDD70F9F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="140" windowWidth="12980" windowHeight="10850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Erledigt?</t>
   </si>
@@ -110,6 +111,9 @@
   </si>
   <si>
     <t>Shallow-Copy &amp; Deep-Copy</t>
+  </si>
+  <si>
+    <t>Data3</t>
   </si>
 </sst>
 </file>
@@ -328,7 +332,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -381,6 +384,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -789,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -798,7 +802,7 @@
     <col min="1" max="1" width="1.26953125" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55.36328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="33.81640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.81640625" style="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.81640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="5.81640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="1" customWidth="1"/>
@@ -806,14 +810,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="9"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="3" spans="2:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="27"/>
+      <c r="D4" s="26"/>
     </row>
     <row r="5" spans="2:5" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -825,7 +829,7 @@
       <c r="D5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>13</v>
       </c>
     </row>
@@ -833,11 +837,11 @@
       <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="16" t="s">
+      <c r="D6" s="20"/>
+      <c r="E6" s="15" t="s">
         <v>14</v>
       </c>
     </row>
@@ -845,76 +849,78 @@
       <c r="B7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="17" t="s">
+      <c r="D7" s="21"/>
+      <c r="E7" s="16" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="13.5" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="16"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="15"/>
     </row>
     <row r="9" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="17"/>
+      <c r="E9" s="16"/>
     </row>
     <row r="10" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="16"/>
+      <c r="E10" s="15" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="17"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="16"/>
     </row>
     <row r="12" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="16"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="15"/>
     </row>
     <row r="13" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="16"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="20"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="19"/>
     </row>
     <row r="15" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="28"/>
+      <c r="D15" s="27"/>
     </row>
     <row r="16" spans="2:5" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
@@ -926,145 +932,145 @@
       <c r="D16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="16"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="15"/>
     </row>
     <row r="18" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="17"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="16"/>
     </row>
     <row r="19" spans="2:5" ht="25" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="16"/>
+      <c r="E19" s="15"/>
     </row>
     <row r="20" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="22"/>
-      <c r="E20" s="17"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="16"/>
     </row>
     <row r="21" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="16"/>
+      <c r="E21" s="15"/>
     </row>
     <row r="22" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="17"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="16"/>
     </row>
     <row r="23" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="16"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="15"/>
     </row>
     <row r="24" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="17"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="16"/>
     </row>
     <row r="25" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="18"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="17"/>
     </row>
     <row r="26" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
-      <c r="D26" s="29"/>
+      <c r="D26" s="28"/>
     </row>
     <row r="27" spans="2:5" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="15"/>
+      <c r="E27" s="14"/>
     </row>
     <row r="28" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="16"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="15"/>
     </row>
     <row r="29" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="17"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="16"/>
     </row>
     <row r="30" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="16"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="15"/>
     </row>
     <row r="31" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="17"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="16"/>
     </row>
     <row r="32" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="16"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="15"/>
     </row>
     <row r="33" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="17"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="16"/>
     </row>
     <row r="34" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="16"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="15"/>
     </row>
     <row r="35" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="17"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="16"/>
     </row>
     <row r="36" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="17"/>
     </row>
   </sheetData>
   <autoFilter ref="B5:B30" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
DataArray und TestDataArray eingefügt
</commit_message>
<xml_diff>
--- a/Aufgabenliste.xlsx
+++ b/Aufgabenliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\workspace\JavaMemoryTracerAufgaben\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF7A04E-99F1-42A2-A29C-509970D2054F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479376CF-9588-450F-BDBB-122F4A81C868}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="140" windowWidth="12980" windowHeight="10850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Erledigt?</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>Data4</t>
+  </si>
+  <si>
+    <t>wurde in Data3 mit behandelt</t>
+  </si>
+  <si>
+    <t>DataArray</t>
   </si>
 </sst>
 </file>
@@ -185,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -307,11 +313,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -362,12 +388,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -377,16 +397,19 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -797,7 +820,7 @@
   <dimension ref="B1:E36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -805,7 +828,7 @@
     <col min="1" max="1" width="1.26953125" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55.36328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="33.81640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.81640625" style="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.81640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="5.81640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="1" customWidth="1"/>
@@ -813,14 +836,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="28"/>
     </row>
     <row r="3" spans="2:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="26"/>
+      <c r="D4" s="23"/>
     </row>
     <row r="5" spans="2:5" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -843,7 +866,7 @@
       <c r="C6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="18"/>
       <c r="E6" s="15" t="s">
         <v>14</v>
       </c>
@@ -855,7 +878,7 @@
       <c r="C7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="21"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="16" t="s">
         <v>15</v>
       </c>
@@ -867,7 +890,7 @@
       <c r="C8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="20" t="s">
         <v>19</v>
       </c>
       <c r="E8" s="15" t="s">
@@ -879,7 +902,7 @@
       <c r="C9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="19" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="16"/>
@@ -891,45 +914,53 @@
       <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7"/>
+    <row r="11" spans="2:5" ht="25" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="C11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="16"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="16" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="C12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="15"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="15" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="15"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="16"/>
     </row>
     <row r="14" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="19"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="17"/>
     </row>
     <row r="15" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="27"/>
+      <c r="D15" s="25"/>
     </row>
     <row r="16" spans="2:5" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
@@ -950,7 +981,7 @@
       <c r="C17" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="20"/>
+      <c r="D17" s="18"/>
       <c r="E17" s="15"/>
     </row>
     <row r="18" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -958,7 +989,7 @@
       <c r="C18" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="21"/>
+      <c r="D18" s="19"/>
       <c r="E18" s="16"/>
     </row>
     <row r="19" spans="2:5" ht="25" x14ac:dyDescent="0.25">
@@ -966,7 +997,7 @@
       <c r="C19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="20" t="s">
         <v>26</v>
       </c>
       <c r="E19" s="15"/>
@@ -976,7 +1007,7 @@
       <c r="C20" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="21"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="16"/>
     </row>
     <row r="21" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -984,7 +1015,7 @@
       <c r="C21" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="20" t="s">
         <v>27</v>
       </c>
       <c r="E21" s="15"/>
@@ -994,7 +1025,7 @@
       <c r="C22" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="21"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="16"/>
     </row>
     <row r="23" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1002,24 +1033,24 @@
       <c r="C23" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="22"/>
+      <c r="D23" s="20"/>
       <c r="E23" s="15"/>
     </row>
     <row r="24" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="21"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="16"/>
     </row>
     <row r="25" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="11"/>
-      <c r="D25" s="24"/>
+      <c r="D25" s="21"/>
       <c r="E25" s="17"/>
     </row>
     <row r="26" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
-      <c r="D26" s="28"/>
+      <c r="D26" s="24"/>
     </row>
     <row r="27" spans="2:5" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
@@ -1030,55 +1061,55 @@
     <row r="28" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="C28" s="12"/>
-      <c r="D28" s="20"/>
+      <c r="D28" s="18"/>
       <c r="E28" s="15"/>
     </row>
     <row r="29" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="9"/>
-      <c r="D29" s="21"/>
+      <c r="D29" s="19"/>
       <c r="E29" s="16"/>
     </row>
     <row r="30" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="C30" s="12"/>
-      <c r="D30" s="22"/>
+      <c r="D30" s="20"/>
       <c r="E30" s="15"/>
     </row>
     <row r="31" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
       <c r="C31" s="9"/>
-      <c r="D31" s="21"/>
+      <c r="D31" s="19"/>
       <c r="E31" s="16"/>
     </row>
     <row r="32" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7"/>
       <c r="C32" s="12"/>
-      <c r="D32" s="22"/>
+      <c r="D32" s="20"/>
       <c r="E32" s="15"/>
     </row>
     <row r="33" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="C33" s="9"/>
-      <c r="D33" s="21"/>
+      <c r="D33" s="19"/>
       <c r="E33" s="16"/>
     </row>
     <row r="34" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="C34" s="12"/>
-      <c r="D34" s="22"/>
+      <c r="D34" s="20"/>
       <c r="E34" s="15"/>
     </row>
     <row r="35" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
       <c r="C35" s="9"/>
-      <c r="D35" s="21"/>
+      <c r="D35" s="19"/>
       <c r="E35" s="16"/>
     </row>
     <row r="36" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="7"/>
       <c r="C36" s="13"/>
-      <c r="D36" s="24"/>
+      <c r="D36" s="21"/>
       <c r="E36" s="17"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MethAttr und TestMethAttr hinzugefügt
</commit_message>
<xml_diff>
--- a/Aufgabenliste.xlsx
+++ b/Aufgabenliste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\workspace\JavaMemoryTracerAufgaben\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479376CF-9588-450F-BDBB-122F4A81C868}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BB937E-2103-474C-BD03-58888AB967B9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="140" windowWidth="12980" windowHeight="10850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>Erledigt?</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>DataArray</t>
+  </si>
+  <si>
+    <t>Meth1</t>
+  </si>
+  <si>
+    <t>MethAttr</t>
   </si>
 </sst>
 </file>
@@ -819,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -977,20 +983,28 @@
       </c>
     </row>
     <row r="17" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
+      <c r="B17" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="C17" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D17" s="18"/>
-      <c r="E17" s="15"/>
+      <c r="E17" s="15" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="18" spans="2:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
+      <c r="B18" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="C18" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="19"/>
-      <c r="E18" s="16"/>
+      <c r="E18" s="16" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="19" spans="2:5" ht="25" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>

</xml_diff>

<commit_message>
MethAttr vereinfacht, MethConstr eingefügt (besteht Test noch nicht)
</commit_message>
<xml_diff>
--- a/Aufgabenliste.xlsx
+++ b/Aufgabenliste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\workspace\JavaMemoryTracerAufgaben\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BB937E-2103-474C-BD03-58888AB967B9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6392A72-B1DC-4E03-867C-E2F558B87F1B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="140" windowWidth="12980" windowHeight="10850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Erledigt?</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>MethAttr</t>
+  </si>
+  <si>
+    <t>t</t>
   </si>
 </sst>
 </file>
@@ -826,7 +829,7 @@
   <dimension ref="B1:E36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1007,7 +1010,9 @@
       </c>
     </row>
     <row r="19" spans="2:5" ht="25" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
+      <c r="B19" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="C19" s="10" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Aufgabenliste geupdated, MethCopy eingefügt (fails)
</commit_message>
<xml_diff>
--- a/Aufgabenliste.xlsx
+++ b/Aufgabenliste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\workspace\JavaMemoryTracerAufgaben\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C85A6BB-7128-409A-8747-0F65844A26DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6197F9-4660-4992-B007-2807483C703E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="365" yWindow="140" windowWidth="12981" windowHeight="10854" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Erledigt?</t>
   </si>
@@ -125,13 +125,19 @@
     <t>MethAttr</t>
   </si>
   <si>
-    <t>r</t>
-  </si>
-  <si>
     <t>wird fürs erste nicht bearbeitet, da der Memory Tracer nicht mit static-Attributen klar kommt</t>
   </si>
   <si>
     <t>Konstruktoren &amp; Konstruktor-Verkettung</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>MethConstr</t>
+  </si>
+  <si>
+    <t>MethEquals</t>
   </si>
 </sst>
 </file>
@@ -828,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="12.9" x14ac:dyDescent="0.25"/>
@@ -1014,22 +1020,24 @@
         <v>2</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="15"/>
+      <c r="E19" s="15" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="20" spans="2:5" ht="38.700000000000003" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>23</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E20" s="16"/>
     </row>
@@ -1043,10 +1051,14 @@
       <c r="D21" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="15"/>
+      <c r="E21" s="15" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="22" spans="2:5" ht="16.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
+      <c r="B22" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="C22" s="9" t="s">
         <v>26</v>
       </c>

</xml_diff>